<commit_message>
-Fix the LEDs quantity in the BOM
</commit_message>
<xml_diff>
--- a/Released/BOM/H16R6.xlsx
+++ b/Released/BOM/H16R6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H16R6x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7E8E90-DF68-4CBE-B0D1-521E99C41ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5382322-8C6C-44D9-84BB-849D094E558F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H16R6" sheetId="1" r:id="rId1"/>
@@ -634,9 +634,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2277741</xdr:colOff>
+      <xdr:colOff>2275836</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>20002</xdr:rowOff>
+      <xdr:rowOff>16192</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -977,7 +977,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:D22"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1333,7 @@
         <v>84</v>
       </c>
       <c r="F20" s="19">
-        <v>6.4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edit the logo Add the TVS diode
</commit_message>
<xml_diff>
--- a/Released/BOM/H16R6.xlsx
+++ b/Released/BOM/H16R6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H16R6x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5382322-8C6C-44D9-84BB-849D094E558F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D411E6E4-7113-420A-B2BD-EDE2B31C8294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2640" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H16R6" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
   <si>
     <t>Description</t>
   </si>
@@ -323,6 +323,21 @@
   </si>
   <si>
     <t>Voltage Level Translator 2-CH Bidirectional 8-Pin X2-DFN T/R</t>
+  </si>
+  <si>
+    <t>TVS DIODE 3,3V 10,9V SOD323</t>
+  </si>
+  <si>
+    <t>CDSOD323-T03SC</t>
+  </si>
+  <si>
+    <t>BOURNS INC</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cdsod323-t03sc-bourns-10487153?r=sp</t>
+  </si>
+  <si>
+    <t>D66</t>
   </si>
 </sst>
 </file>
@@ -522,7 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -598,6 +613,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -634,7 +661,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2275836</xdr:colOff>
+      <xdr:colOff>2270121</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>16192</xdr:rowOff>
     </xdr:to>
@@ -974,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1336,41 +1363,41 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="19">
+    <row r="21" spans="1:6" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>87</v>
+        <v>25</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="F22" s="19">
         <v>1</v>
@@ -1378,21 +1405,41 @@
     </row>
     <row r="23" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B24" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C24" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D24" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E24" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F24" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1403,8 +1450,8 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E23" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E24" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="D19" r:id="rId3" display="https://octopart.com/manufacturers/wolfspeed" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="E18" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>

</xml_diff>

<commit_message>
Replace the led APA-102-2020-6 with APA-102-2020-8
</commit_message>
<xml_diff>
--- a/Released/BOM/H16R6.xlsx
+++ b/Released/BOM/H16R6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H16R6x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF819BE6-488D-497E-B52F-64E8FEF7ACDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D411E6E4-7113-420A-B2BD-EDE2B31C8294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2640" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H16R6" sheetId="1" r:id="rId1"/>
@@ -257,6 +257,9 @@
     <t>D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15, D16, D17, D18, D19, D20, D21, D22, D23, D24, D25, D26, D27, D28, D29, D30, D31, D32, D33, D34, D35, D36, D37, D38, D39, D40, D41, D42, D43, D44, D45, D46, D47, D48, D49, D50, D51, D52, D53, D54, D55, D56, D57, D58, D59, D60, D61, D62, D63, D64, D65</t>
   </si>
   <si>
+    <t>C1, C3, C5, C6, C8, C10, C11, C12, C13, C14, C15, C17, C18, C19, C21, C22, C30, C31, C32</t>
+  </si>
+  <si>
     <t>C7, C4, C9, C16, C20, C23, C24, C25, C26, C27</t>
   </si>
   <si>
@@ -335,9 +338,6 @@
   </si>
   <si>
     <t>D66</t>
-  </si>
-  <si>
-    <t>C3, C5, C6, C8, C10, C11, C12, C13, C14, C15, C17, C18, C19, C21, C22, C30, C31, C32</t>
   </si>
 </sst>
 </file>
@@ -593,6 +593,27 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,27 +625,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1064,11 +1064,11 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="21">
         <v>0</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1081,11 +1081,11 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="22">
         <v>45332</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1098,9 +1098,9 @@
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="31"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1125,7 +1125,7 @@
     </row>
     <row r="9" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>42</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="10" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>43</v>
@@ -1165,19 +1165,19 @@
     </row>
     <row r="11" spans="1:9" s="16" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F11" s="19">
         <v>4</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="12" spans="1:9" s="16" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>51</v>
@@ -1200,7 +1200,7 @@
         <v>53</v>
       </c>
       <c r="F12" s="19">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1225,7 +1225,7 @@
     </row>
     <row r="14" spans="1:9" s="16" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>54</v>
@@ -1348,38 +1348,38 @@
         <v>72</v>
       </c>
       <c r="B20" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>84</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>83</v>
       </c>
       <c r="F20" s="19">
         <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="21" t="s">
+      <c r="A21" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" s="24">
+      <c r="F21" s="31">
         <v>1</v>
       </c>
     </row>
@@ -1408,16 +1408,16 @@
         <v>70</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>71</v>
       </c>
       <c r="D23" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="18" t="s">
         <v>86</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>85</v>
       </c>
       <c r="F23" s="19">
         <v>1</v>

</xml_diff>

<commit_message>
Fix the clearance and soldermask issues Replace the 0603 4.7uF tant cap with ceramic cap in the BOM
</commit_message>
<xml_diff>
--- a/Released/BOM/H16R6.xlsx
+++ b/Released/BOM/H16R6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H16R6x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D411E6E4-7113-420A-B2BD-EDE2B31C8294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C339C5A2-437B-4532-9535-3C9FA544E06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2640" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H16R6" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="93">
   <si>
     <t>Description</t>
   </si>
@@ -200,18 +200,6 @@
     <t>https://octopart.com/cga2b1x7r1c104k050bc-tdk-26014376?r=sp</t>
   </si>
   <si>
-    <t>Tantalum Capacitors - Polymer 4.7uF 10V 20% 0603 ESR=500 mOhm</t>
-  </si>
-  <si>
-    <t>F381A475MMA</t>
-  </si>
-  <si>
-    <t>KYOCERA AVX</t>
-  </si>
-  <si>
-    <t>https://octopart.com/f381a475mma-kyocera+avx-122115684?r=sp</t>
-  </si>
-  <si>
     <t>CAP CER 1UF 10V X5R 0402</t>
   </si>
   <si>
@@ -255,9 +243,6 @@
   </si>
   <si>
     <t>D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13, D14, D15, D16, D17, D18, D19, D20, D21, D22, D23, D24, D25, D26, D27, D28, D29, D30, D31, D32, D33, D34, D35, D36, D37, D38, D39, D40, D41, D42, D43, D44, D45, D46, D47, D48, D49, D50, D51, D52, D53, D54, D55, D56, D57, D58, D59, D60, D61, D62, D63, D64, D65</t>
-  </si>
-  <si>
-    <t>C1, C3, C5, C6, C8, C10, C11, C12, C13, C14, C15, C17, C18, C19, C21, C22, C30, C31, C32</t>
   </si>
   <si>
     <t>C7, C4, C9, C16, C20, C23, C24, C25, C26, C27</t>
@@ -338,6 +323,18 @@
   </si>
   <si>
     <t>D66</t>
+  </si>
+  <si>
+    <t>C3, C5, C6, C8, C10, C11, C12, C13, C14, C15, C17, C18, C19, C21, C22, C30, C31, C32</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 25V 4.7uF X5R 10% T: 0.8mm</t>
+  </si>
+  <si>
+    <t>C1608X5R1E475K080AC</t>
+  </si>
+  <si>
+    <t>https://octopart.com/c1608x5r1e475k080ac-tdk-26013502?r=sp</t>
   </si>
 </sst>
 </file>
@@ -537,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -593,6 +590,18 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -614,17 +623,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1003,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1064,11 +1064,11 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="25">
         <v>0</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1081,11 +1081,11 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="26">
         <v>45332</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1093,14 +1093,14 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="31"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
@@ -1125,7 +1125,7 @@
     </row>
     <row r="9" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>42</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="10" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>43</v>
@@ -1165,19 +1165,19 @@
     </row>
     <row r="11" spans="1:9" s="16" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F11" s="19">
         <v>4</v>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="12" spans="1:9" s="16" customFormat="1" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>51</v>
@@ -1200,7 +1200,7 @@
         <v>53</v>
       </c>
       <c r="F12" s="19">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -1208,16 +1208,16 @@
         <v>36</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>44</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F13" s="19">
         <v>1</v>
@@ -1225,19 +1225,19 @@
     </row>
     <row r="14" spans="1:9" s="16" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>57</v>
+        <v>38</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>92</v>
       </c>
       <c r="F14" s="19">
         <v>10</v>
@@ -1245,7 +1245,7 @@
     </row>
     <row r="15" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>47</v>
@@ -1268,16 +1268,16 @@
         <v>33</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F16" s="19">
         <v>1</v>
@@ -1285,19 +1285,19 @@
     </row>
     <row r="17" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F17" s="19">
         <v>3</v>
@@ -1345,41 +1345,41 @@
     </row>
     <row r="20" spans="1:6" s="16" customFormat="1" ht="277.2" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F20" s="19">
         <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" s="31">
+      <c r="A21" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="24">
         <v>1</v>
       </c>
     </row>
@@ -1405,19 +1405,19 @@
     </row>
     <row r="23" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F23" s="19">
         <v>1</v>
@@ -1458,7 +1458,7 @@
     <hyperlink ref="E19" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
     <hyperlink ref="E15" r:id="rId7" display="https://octopart.com/rc0603jr-070rl-yageo-1241539?r=sp" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="E12" r:id="rId8" display="https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g" xr:uid="{663B604C-0778-4D31-8D01-1E3B83AE8D9B}"/>
-    <hyperlink ref="E14" r:id="rId9" display="https://octopart.com/10tpu4r7msi-panasonic-29487748?r=sp" xr:uid="{23CC8D52-00B7-424D-AE6F-D90CF0F8A6D7}"/>
+    <hyperlink ref="E14" r:id="rId9" xr:uid="{23CC8D52-00B7-424D-AE6F-D90CF0F8A6D7}"/>
     <hyperlink ref="E16" r:id="rId10" display="https://octopart.com/erj-3geyj271v-panasonic-55560546" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="E17" r:id="rId11" display="https://octopart.com/search?q=RC0603FR-0710KL&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E9" r:id="rId12" display="https://octopart.com/87227-1-te+connectivity-39512052?r=sp" xr:uid="{97DC24F0-08CA-4316-A0CB-F81F9DEADBAB}"/>

</xml_diff>